<commit_message>
Add Dockerfile and requirements for frontend and backend integration
</commit_message>
<xml_diff>
--- a/chatkit/Rent_Workbook_2025.xlsx
+++ b/chatkit/Rent_Workbook_2025.xlsx
@@ -1370,7 +1370,7 @@
       </c>
       <c r="I9" s="18" t="inlineStr">
         <is>
-          <t>($3925) fr 2024 + $2641 Jan= $6566.  Dee pd $200</t>
+          <t>($3925) fr 2024 + $2641 Jan= $6566. , Dee pd $200</t>
         </is>
       </c>
     </row>
@@ -3259,17 +3259,21 @@
         </is>
       </c>
       <c r="B20" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="inlineStr"/>
+        <v>2775</v>
+      </c>
+      <c r="C20" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D20" s="16" t="n">
-        <v>0</v>
+        <v>2775</v>
       </c>
       <c r="E20" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="16" t="n">
-        <v>0</v>
+        <v>2775</v>
       </c>
       <c r="G20" s="67" t="n">
         <v>0</v>
@@ -3277,11 +3281,7 @@
       <c r="H20" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I20" s="18" t="inlineStr"/>
     </row>
     <row r="21" ht="22" customHeight="1" thickBot="1">
       <c r="A21" s="20" t="inlineStr">
@@ -3467,7 +3467,11 @@
           <t>Property:</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>2701 Echo Point Dr.</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
@@ -3477,7 +3481,11 @@
         </is>
       </c>
       <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="inlineStr"/>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Kristine Zepeda</t>
+        </is>
+      </c>
       <c r="I4" s="5" t="n"/>
     </row>
     <row r="5" ht="19" customHeight="1">
@@ -3585,27 +3593,31 @@
         </is>
       </c>
       <c r="B9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="inlineStr"/>
+        <v>5828</v>
+      </c>
+      <c r="C9" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D9" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="E9" s="16" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>0</v>
+        <v>2121</v>
       </c>
       <c r="G9" s="67" t="n">
-        <v>0</v>
+        <v>-3707</v>
       </c>
       <c r="H9" s="67" t="n">
-        <v>0</v>
+        <v>-3707</v>
       </c>
       <c r="I9" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>$3128 (2024 under bal) + Rent $2700 = $5828 T pd $150</t>
         </is>
       </c>
     </row>
@@ -3616,29 +3628,29 @@
         </is>
       </c>
       <c r="B10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C10" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D10" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="E10" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="G10" s="67" t="n">
-        <v>0</v>
+        <v>-729</v>
       </c>
       <c r="H10" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+        <v>-4436</v>
+      </c>
+      <c r="I10" s="18" t="inlineStr"/>
     </row>
     <row r="11" ht="22" customHeight="1">
       <c r="A11" s="13" t="inlineStr">
@@ -3647,29 +3659,29 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D11" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="E11" s="16" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>0</v>
+        <v>2471</v>
       </c>
       <c r="G11" s="67" t="n">
-        <v>0</v>
+        <v>-229</v>
       </c>
       <c r="H11" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+        <v>-4665</v>
+      </c>
+      <c r="I11" s="18" t="inlineStr"/>
     </row>
     <row r="12" ht="22" customHeight="1">
       <c r="A12" s="13" t="inlineStr">
@@ -3678,29 +3690,29 @@
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D12" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="E12" s="16" t="n">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>0</v>
+        <v>2701</v>
       </c>
       <c r="G12" s="67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+        <v>-4664</v>
+      </c>
+      <c r="I12" s="18" t="inlineStr"/>
     </row>
     <row r="13" ht="22" customHeight="1">
       <c r="A13" s="13" t="inlineStr">
@@ -3709,29 +3721,29 @@
         </is>
       </c>
       <c r="B13" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C13" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D13" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="E13" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="G13" s="67" t="n">
-        <v>0</v>
+        <v>-729</v>
       </c>
       <c r="H13" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+        <v>-5393</v>
+      </c>
+      <c r="I13" s="18" t="inlineStr"/>
     </row>
     <row r="14" ht="22" customHeight="1">
       <c r="A14" s="13" t="inlineStr">
@@ -3740,29 +3752,29 @@
         </is>
       </c>
       <c r="B14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C14" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D14" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="E14" s="16" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>0</v>
+        <v>2171</v>
       </c>
       <c r="G14" s="67" t="n">
-        <v>0</v>
+        <v>-529</v>
       </c>
       <c r="H14" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+        <v>-5922</v>
+      </c>
+      <c r="I14" s="18" t="inlineStr"/>
     </row>
     <row r="15" ht="22" customHeight="1">
       <c r="A15" s="13" t="inlineStr">
@@ -3771,29 +3783,29 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C15" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D15" s="16" t="n">
-        <v>0</v>
+        <v>1971</v>
       </c>
       <c r="E15" s="16" t="n">
-        <v>0</v>
+        <v>201.5</v>
       </c>
       <c r="F15" s="16" t="n">
-        <v>0</v>
+        <v>2172.5</v>
       </c>
       <c r="G15" s="67" t="n">
-        <v>0</v>
+        <v>-527.5</v>
       </c>
       <c r="H15" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+        <v>-6449.5</v>
+      </c>
+      <c r="I15" s="18" t="inlineStr"/>
     </row>
     <row r="16" ht="22" customHeight="1">
       <c r="A16" s="13" t="inlineStr">
@@ -3802,27 +3814,31 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C16" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D16" s="16" t="n">
-        <v>0</v>
+        <v>2510</v>
       </c>
       <c r="E16" s="16" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F16" s="16" t="n">
-        <v>0</v>
+        <v>2710</v>
       </c>
       <c r="G16" s="67" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H16" s="67" t="n">
-        <v>0</v>
+        <v>-6439.5</v>
       </c>
       <c r="I16" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Eff 8/1 (HS: $2510 + T: $190) T pd $200 9/2</t>
         </is>
       </c>
     </row>
@@ -3833,27 +3849,31 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C17" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D17" s="16" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="16" t="n">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="F17" s="16" t="n">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="G17" s="67" t="n">
-        <v>0</v>
+        <v>-2510</v>
       </c>
       <c r="H17" s="67" t="n">
-        <v>0</v>
+        <v>-8949.5</v>
       </c>
       <c r="I17" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>THS pd ($2510) 2 = $5020</t>
         </is>
       </c>
     </row>
@@ -3864,27 +3884,31 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="inlineStr"/>
+        <v>2700</v>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D18" s="16" t="n">
-        <v>0</v>
+        <v>5020</v>
       </c>
       <c r="E18" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="16" t="n">
-        <v>0</v>
+        <v>5020</v>
       </c>
       <c r="G18" s="67" t="n">
-        <v>0</v>
+        <v>2320</v>
       </c>
       <c r="H18" s="67" t="n">
-        <v>0</v>
+        <v>-6629.5</v>
       </c>
       <c r="I18" s="19" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>THS pd ($2510) 2 = $5020</t>
         </is>
       </c>
     </row>
@@ -3895,9 +3919,13 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15" t="inlineStr"/>
+        <v>2250</v>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D19" s="16" t="n">
         <v>0</v>
       </c>
@@ -3908,14 +3936,14 @@
         <v>0</v>
       </c>
       <c r="G19" s="67" t="n">
-        <v>0</v>
+        <v>-2250</v>
       </c>
       <c r="H19" s="67" t="n">
-        <v>0</v>
+        <v>-8879.5</v>
       </c>
       <c r="I19" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Housing Terminated contract Oct 31, 2025   25 days x $90 = $2,250 (Nov)</t>
         </is>
       </c>
     </row>
@@ -3928,7 +3956,11 @@
       <c r="B20" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="15" t="inlineStr"/>
+      <c r="C20" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D20" s="16" t="n">
         <v>0</v>
       </c>
@@ -3942,13 +3974,9 @@
         <v>0</v>
       </c>
       <c r="H20" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+        <v>-8879.5</v>
+      </c>
+      <c r="I20" s="18" t="inlineStr"/>
     </row>
     <row r="21" ht="22" customHeight="1" thickBot="1">
       <c r="A21" s="20" t="inlineStr">
@@ -4134,7 +4162,11 @@
           <t>Property:</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>2604 Poplar Springs</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
@@ -4144,7 +4176,11 @@
         </is>
       </c>
       <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="inlineStr"/>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Sandra Flory</t>
+        </is>
+      </c>
       <c r="I4" s="5" t="n"/>
     </row>
     <row r="5" ht="19" customHeight="1">
@@ -4252,17 +4288,21 @@
         </is>
       </c>
       <c r="B9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C9" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D9" s="16" t="n">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="E9" s="16" t="n">
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G9" s="67" t="n">
         <v>0</v>
@@ -4270,11 +4310,7 @@
       <c r="H9" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I9" s="18" t="inlineStr"/>
     </row>
     <row r="10" ht="22" customHeight="1">
       <c r="A10" s="13" t="inlineStr">
@@ -4283,17 +4319,21 @@
         </is>
       </c>
       <c r="B10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C10" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D10" s="16" t="n">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="E10" s="16" t="n">
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G10" s="67" t="n">
         <v>0</v>
@@ -4301,11 +4341,7 @@
       <c r="H10" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I10" s="18" t="inlineStr"/>
     </row>
     <row r="11" ht="22" customHeight="1">
       <c r="A11" s="13" t="inlineStr">
@@ -4314,17 +4350,21 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D11" s="16" t="n">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="E11" s="16" t="n">
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G11" s="67" t="n">
         <v>0</v>
@@ -4332,11 +4372,7 @@
       <c r="H11" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I11" s="18" t="inlineStr"/>
     </row>
     <row r="12" ht="22" customHeight="1">
       <c r="A12" s="13" t="inlineStr">
@@ -4345,17 +4381,21 @@
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D12" s="16" t="n">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="E12" s="16" t="n">
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G12" s="67" t="n">
         <v>0</v>
@@ -4365,7 +4405,7 @@
       </c>
       <c r="I12" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>T pd: $1000 4/2 + $236 $/4/3 = $1,236</t>
         </is>
       </c>
     </row>
@@ -4376,17 +4416,21 @@
         </is>
       </c>
       <c r="B13" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C13" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D13" s="16" t="n">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="E13" s="16" t="n">
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G13" s="67" t="n">
         <v>0</v>
@@ -4394,11 +4438,7 @@
       <c r="H13" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I13" s="18" t="inlineStr"/>
     </row>
     <row r="14" ht="22" customHeight="1">
       <c r="A14" s="13" t="inlineStr">
@@ -4407,17 +4447,21 @@
         </is>
       </c>
       <c r="B14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C14" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D14" s="16" t="n">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="E14" s="16" t="n">
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G14" s="67" t="n">
         <v>0</v>
@@ -4425,11 +4469,7 @@
       <c r="H14" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I14" s="18" t="inlineStr"/>
     </row>
     <row r="15" ht="22" customHeight="1">
       <c r="A15" s="13" t="inlineStr">
@@ -4438,17 +4478,21 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C15" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D15" s="16" t="n">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="E15" s="16" t="n">
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="F15" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G15" s="67" t="n">
         <v>0</v>
@@ -4456,11 +4500,7 @@
       <c r="H15" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I15" s="18" t="inlineStr"/>
     </row>
     <row r="16" ht="22" customHeight="1">
       <c r="A16" s="13" t="inlineStr">
@@ -4469,17 +4509,21 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C16" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D16" s="16" t="n">
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="E16" s="16" t="n">
-        <v>0</v>
+        <v>1236</v>
       </c>
       <c r="F16" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G16" s="67" t="n">
         <v>0</v>
@@ -4487,11 +4531,7 @@
       <c r="H16" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I16" s="18" t="inlineStr"/>
     </row>
     <row r="17" ht="22" customHeight="1">
       <c r="A17" s="13" t="inlineStr">
@@ -4500,17 +4540,21 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C17" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D17" s="16" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="E17" s="16" t="n">
-        <v>0</v>
+        <v>774</v>
       </c>
       <c r="F17" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G17" s="67" t="n">
         <v>0</v>
@@ -4520,7 +4564,7 @@
       </c>
       <c r="I17" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Eff 9/1 (HS: $2,008 + T: $774), T pd $774</t>
         </is>
       </c>
     </row>
@@ -4531,17 +4575,21 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D18" s="16" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="E18" s="16" t="n">
-        <v>0</v>
+        <v>774</v>
       </c>
       <c r="F18" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G18" s="67" t="n">
         <v>0</v>
@@ -4549,11 +4597,7 @@
       <c r="H18" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="19" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I18" s="19" t="inlineStr"/>
     </row>
     <row r="19" ht="22" customHeight="1">
       <c r="A19" s="13" t="inlineStr">
@@ -4562,17 +4606,21 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D19" s="16" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="E19" s="16" t="n">
-        <v>0</v>
+        <v>774</v>
       </c>
       <c r="F19" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G19" s="67" t="n">
         <v>0</v>
@@ -4580,11 +4628,7 @@
       <c r="H19" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I19" s="18" t="inlineStr"/>
     </row>
     <row r="20" ht="22" customHeight="1">
       <c r="A20" s="13" t="inlineStr">
@@ -4593,17 +4637,21 @@
         </is>
       </c>
       <c r="B20" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="inlineStr"/>
+        <v>2782</v>
+      </c>
+      <c r="C20" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D20" s="16" t="n">
-        <v>0</v>
+        <v>2008</v>
       </c>
       <c r="E20" s="16" t="n">
-        <v>0</v>
+        <v>774</v>
       </c>
       <c r="F20" s="16" t="n">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="G20" s="67" t="n">
         <v>0</v>
@@ -4611,11 +4659,7 @@
       <c r="H20" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I20" s="18" t="inlineStr"/>
     </row>
     <row r="21" ht="22" customHeight="1" thickBot="1">
       <c r="A21" s="20" t="inlineStr">
@@ -4801,7 +4845,11 @@
           <t>Property:</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>2817 Country Creek</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
@@ -4811,7 +4859,11 @@
         </is>
       </c>
       <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="inlineStr"/>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Alisha Friddle</t>
+        </is>
+      </c>
       <c r="I4" s="5" t="n"/>
     </row>
     <row r="5" ht="19" customHeight="1">
@@ -4919,17 +4971,21 @@
         </is>
       </c>
       <c r="B9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C9" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D9" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="E9" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="G9" s="67" t="n">
         <v>0</v>
@@ -4937,11 +4993,7 @@
       <c r="H9" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I9" s="18" t="inlineStr"/>
     </row>
     <row r="10" ht="22" customHeight="1">
       <c r="A10" s="13" t="inlineStr">
@@ -4950,17 +5002,21 @@
         </is>
       </c>
       <c r="B10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C10" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D10" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="E10" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="G10" s="67" t="n">
         <v>0</v>
@@ -4968,11 +5024,7 @@
       <c r="H10" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I10" s="18" t="inlineStr"/>
     </row>
     <row r="11" ht="22" customHeight="1">
       <c r="A11" s="13" t="inlineStr">
@@ -4981,17 +5033,21 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D11" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="E11" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="G11" s="67" t="n">
         <v>0</v>
@@ -4999,11 +5055,7 @@
       <c r="H11" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I11" s="18" t="inlineStr"/>
     </row>
     <row r="12" ht="22" customHeight="1">
       <c r="A12" s="13" t="inlineStr">
@@ -5012,17 +5064,21 @@
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D12" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="E12" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="G12" s="67" t="n">
         <v>0</v>
@@ -5030,11 +5086,7 @@
       <c r="H12" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I12" s="18" t="inlineStr"/>
     </row>
     <row r="13" ht="22" customHeight="1">
       <c r="A13" s="13" t="inlineStr">
@@ -5043,17 +5095,21 @@
         </is>
       </c>
       <c r="B13" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C13" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D13" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="E13" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="G13" s="67" t="n">
         <v>0</v>
@@ -5061,11 +5117,7 @@
       <c r="H13" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I13" s="18" t="inlineStr"/>
     </row>
     <row r="14" ht="22" customHeight="1">
       <c r="A14" s="13" t="inlineStr">
@@ -5074,17 +5126,21 @@
         </is>
       </c>
       <c r="B14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C14" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D14" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="E14" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="G14" s="67" t="n">
         <v>0</v>
@@ -5092,11 +5148,7 @@
       <c r="H14" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I14" s="18" t="inlineStr"/>
     </row>
     <row r="15" ht="22" customHeight="1">
       <c r="A15" s="13" t="inlineStr">
@@ -5105,17 +5157,21 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C15" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D15" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="E15" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="G15" s="67" t="n">
         <v>0</v>
@@ -5123,11 +5179,7 @@
       <c r="H15" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I15" s="18" t="inlineStr"/>
     </row>
     <row r="16" ht="22" customHeight="1">
       <c r="A16" s="13" t="inlineStr">
@@ -5136,17 +5188,21 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C16" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D16" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="E16" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F16" s="16" t="n">
-        <v>0</v>
+        <v>2632</v>
       </c>
       <c r="G16" s="67" t="n">
         <v>0</v>
@@ -5154,11 +5210,7 @@
       <c r="H16" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I16" s="18" t="inlineStr"/>
     </row>
     <row r="17" ht="22" customHeight="1">
       <c r="A17" s="13" t="inlineStr">
@@ -5167,27 +5219,31 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C17" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D17" s="16" t="n">
-        <v>0</v>
+        <v>2218</v>
       </c>
       <c r="E17" s="16" t="n">
-        <v>0</v>
+        <v>485</v>
       </c>
       <c r="F17" s="16" t="n">
-        <v>0</v>
+        <v>2703</v>
       </c>
       <c r="G17" s="67" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="H17" s="67" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="I17" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Eff 11/1 (HS: $2,147+ T: $485) , T pd $300 8/28 + $185 9/4 = $485</t>
         </is>
       </c>
     </row>
@@ -5198,27 +5254,31 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D18" s="16" t="n">
-        <v>0</v>
+        <v>2218</v>
       </c>
       <c r="E18" s="16" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F18" s="16" t="n">
-        <v>0</v>
+        <v>2418</v>
       </c>
       <c r="G18" s="67" t="n">
-        <v>0</v>
+        <v>-214</v>
       </c>
       <c r="H18" s="67" t="n">
-        <v>0</v>
+        <v>-143</v>
       </c>
       <c r="I18" s="19" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>HS pd $2147 + $71 = $2218, T pd $200 10/27</t>
         </is>
       </c>
     </row>
@@ -5229,27 +5289,31 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D19" s="16" t="n">
-        <v>0</v>
+        <v>2147</v>
       </c>
       <c r="E19" s="16" t="n">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="F19" s="16" t="n">
-        <v>0</v>
+        <v>2447</v>
       </c>
       <c r="G19" s="67" t="n">
-        <v>0</v>
+        <v>-185</v>
       </c>
       <c r="H19" s="67" t="n">
-        <v>0</v>
+        <v>-328</v>
       </c>
       <c r="I19" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>T pd $300 10/31</t>
         </is>
       </c>
     </row>
@@ -5260,27 +5324,31 @@
         </is>
       </c>
       <c r="B20" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="inlineStr"/>
+        <v>2632</v>
+      </c>
+      <c r="C20" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D20" s="16" t="n">
-        <v>0</v>
+        <v>2147</v>
       </c>
       <c r="E20" s="16" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="F20" s="16" t="n">
-        <v>0</v>
+        <v>2547</v>
       </c>
       <c r="G20" s="67" t="n">
-        <v>0</v>
+        <v>-85</v>
       </c>
       <c r="H20" s="67" t="n">
-        <v>0</v>
+        <v>-413</v>
       </c>
       <c r="I20" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>T pd $400 12/1</t>
         </is>
       </c>
     </row>
@@ -5468,7 +5536,11 @@
           <t>Property:</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>3872 Country Ln</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
@@ -5478,7 +5550,11 @@
         </is>
       </c>
       <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="inlineStr"/>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Kenesha Jackson</t>
+        </is>
+      </c>
       <c r="I4" s="5" t="n"/>
     </row>
     <row r="5" ht="19" customHeight="1">
@@ -5586,17 +5662,21 @@
         </is>
       </c>
       <c r="B9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C9" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D9" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E9" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G9" s="67" t="n">
         <v>0</v>
@@ -5604,11 +5684,7 @@
       <c r="H9" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I9" s="18" t="inlineStr"/>
     </row>
     <row r="10" ht="22" customHeight="1">
       <c r="A10" s="13" t="inlineStr">
@@ -5617,17 +5693,21 @@
         </is>
       </c>
       <c r="B10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C10" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D10" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E10" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G10" s="67" t="n">
         <v>0</v>
@@ -5635,11 +5715,7 @@
       <c r="H10" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I10" s="18" t="inlineStr"/>
     </row>
     <row r="11" ht="22" customHeight="1">
       <c r="A11" s="13" t="inlineStr">
@@ -5648,17 +5724,21 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D11" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E11" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G11" s="67" t="n">
         <v>0</v>
@@ -5666,11 +5746,7 @@
       <c r="H11" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I11" s="18" t="inlineStr"/>
     </row>
     <row r="12" ht="22" customHeight="1">
       <c r="A12" s="13" t="inlineStr">
@@ -5679,17 +5755,21 @@
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D12" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E12" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G12" s="67" t="n">
         <v>0</v>
@@ -5697,11 +5777,7 @@
       <c r="H12" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I12" s="18" t="inlineStr"/>
     </row>
     <row r="13" ht="22" customHeight="1">
       <c r="A13" s="13" t="inlineStr">
@@ -5710,17 +5786,21 @@
         </is>
       </c>
       <c r="B13" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C13" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D13" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E13" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G13" s="67" t="n">
         <v>0</v>
@@ -5728,11 +5808,7 @@
       <c r="H13" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I13" s="18" t="inlineStr"/>
     </row>
     <row r="14" ht="22" customHeight="1">
       <c r="A14" s="13" t="inlineStr">
@@ -5741,17 +5817,21 @@
         </is>
       </c>
       <c r="B14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C14" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D14" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E14" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G14" s="67" t="n">
         <v>0</v>
@@ -5759,11 +5839,7 @@
       <c r="H14" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I14" s="18" t="inlineStr"/>
     </row>
     <row r="15" ht="22" customHeight="1">
       <c r="A15" s="13" t="inlineStr">
@@ -5772,17 +5848,21 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C15" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D15" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E15" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G15" s="67" t="n">
         <v>0</v>
@@ -5790,11 +5870,7 @@
       <c r="H15" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I15" s="18" t="inlineStr"/>
     </row>
     <row r="16" ht="22" customHeight="1">
       <c r="A16" s="13" t="inlineStr">
@@ -5803,17 +5879,21 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C16" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D16" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E16" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F16" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G16" s="67" t="n">
         <v>0</v>
@@ -5821,11 +5901,7 @@
       <c r="H16" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I16" s="18" t="inlineStr"/>
     </row>
     <row r="17" ht="22" customHeight="1">
       <c r="A17" s="13" t="inlineStr">
@@ -5834,17 +5910,21 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C17" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D17" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E17" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G17" s="67" t="n">
         <v>0</v>
@@ -5852,11 +5932,7 @@
       <c r="H17" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I17" s="18" t="inlineStr"/>
     </row>
     <row r="18" ht="22" customHeight="1">
       <c r="A18" s="13" t="inlineStr">
@@ -5865,17 +5941,21 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D18" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="E18" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G18" s="67" t="n">
         <v>0</v>
@@ -5883,11 +5963,7 @@
       <c r="H18" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="19" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I18" s="19" t="inlineStr"/>
     </row>
     <row r="19" ht="22" customHeight="1">
       <c r="A19" s="13" t="inlineStr">
@@ -5896,17 +5972,21 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D19" s="16" t="n">
-        <v>0</v>
+        <v>1742</v>
       </c>
       <c r="E19" s="16" t="n">
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="F19" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G19" s="67" t="n">
         <v>0</v>
@@ -5916,7 +5996,7 @@
       </c>
       <c r="I19" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Eff 11/1 (HS $1742 + T $708) = $2,450, T pd $708 10/24</t>
         </is>
       </c>
     </row>
@@ -5927,17 +6007,21 @@
         </is>
       </c>
       <c r="B20" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="inlineStr"/>
+        <v>2450</v>
+      </c>
+      <c r="C20" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D20" s="16" t="n">
-        <v>0</v>
+        <v>1742</v>
       </c>
       <c r="E20" s="16" t="n">
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="F20" s="16" t="n">
-        <v>0</v>
+        <v>2450</v>
       </c>
       <c r="G20" s="67" t="n">
         <v>0</v>
@@ -5945,11 +6029,7 @@
       <c r="H20" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I20" s="18" t="inlineStr"/>
     </row>
     <row r="21" ht="22" customHeight="1" thickBot="1">
       <c r="A21" s="20" t="inlineStr">
@@ -6135,7 +6215,11 @@
           <t>Property:</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>3841 Country Ln</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
@@ -6145,7 +6229,11 @@
         </is>
       </c>
       <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="inlineStr"/>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Laquita Justice</t>
+        </is>
+      </c>
       <c r="I4" s="5" t="n"/>
     </row>
     <row r="5" ht="19" customHeight="1">
@@ -6253,27 +6341,31 @@
         </is>
       </c>
       <c r="B9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="inlineStr"/>
+        <v>3612</v>
+      </c>
+      <c r="C9" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D9" s="16" t="n">
-        <v>0</v>
+        <v>1548</v>
       </c>
       <c r="E9" s="16" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>0</v>
+        <v>2548</v>
       </c>
       <c r="G9" s="67" t="n">
-        <v>0</v>
+        <v>-1064</v>
       </c>
       <c r="H9" s="67" t="n">
-        <v>0</v>
+        <v>-1064</v>
       </c>
       <c r="I9" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Jan $2,315 + $1297 (2024 bal due) = $3,612      A pd $600 + L pd $400 = $1000</t>
         </is>
       </c>
     </row>
@@ -6284,27 +6376,31 @@
         </is>
       </c>
       <c r="B10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C10" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D10" s="16" t="n">
-        <v>0</v>
+        <v>1548</v>
       </c>
       <c r="E10" s="16" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>0</v>
+        <v>2248</v>
       </c>
       <c r="G10" s="67" t="n">
-        <v>0</v>
+        <v>-67</v>
       </c>
       <c r="H10" s="67" t="n">
-        <v>0</v>
+        <v>-1131</v>
       </c>
       <c r="I10" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>$200 (A pd) + $500 (L pd) = $700</t>
         </is>
       </c>
     </row>
@@ -6315,27 +6411,31 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D11" s="16" t="n">
-        <v>0</v>
+        <v>1548</v>
       </c>
       <c r="E11" s="16" t="n">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>0</v>
+        <v>3048</v>
       </c>
       <c r="G11" s="67" t="n">
-        <v>0</v>
+        <v>733</v>
       </c>
       <c r="H11" s="67" t="n">
-        <v>0</v>
+        <v>-398</v>
       </c>
       <c r="I11" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>$850 (A pd) + $650 (L Pd) = $1,500</t>
         </is>
       </c>
     </row>
@@ -6346,27 +6446,31 @@
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D12" s="16" t="n">
-        <v>0</v>
+        <v>887</v>
       </c>
       <c r="E12" s="16" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>0</v>
+        <v>1887</v>
       </c>
       <c r="G12" s="67" t="n">
-        <v>0</v>
+        <v>-428</v>
       </c>
       <c r="H12" s="67" t="n">
-        <v>0</v>
+        <v>-826</v>
       </c>
       <c r="I12" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Eff 4/1 (HS: 887 + T: $1,428)= $2,315.            A: pd $700 + L: pd $300 = $1000</t>
         </is>
       </c>
     </row>
@@ -6377,27 +6481,31 @@
         </is>
       </c>
       <c r="B13" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C13" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D13" s="16" t="n">
-        <v>0</v>
+        <v>887</v>
       </c>
       <c r="E13" s="16" t="n">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>0</v>
+        <v>1587</v>
       </c>
       <c r="G13" s="67" t="n">
-        <v>0</v>
+        <v>-728</v>
       </c>
       <c r="H13" s="67" t="n">
-        <v>0</v>
+        <v>-1554</v>
       </c>
       <c r="I13" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>$700 (A pd)</t>
         </is>
       </c>
     </row>
@@ -6408,27 +6516,31 @@
         </is>
       </c>
       <c r="B14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C14" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D14" s="16" t="n">
-        <v>0</v>
+        <v>887</v>
       </c>
       <c r="E14" s="16" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>0</v>
+        <v>1487</v>
       </c>
       <c r="G14" s="67" t="n">
-        <v>0</v>
+        <v>-828</v>
       </c>
       <c r="H14" s="67" t="n">
-        <v>0</v>
+        <v>-2382</v>
       </c>
       <c r="I14" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>$600 (A pd 3 x $200)</t>
         </is>
       </c>
     </row>
@@ -6439,27 +6551,31 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C15" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D15" s="16" t="n">
-        <v>0</v>
+        <v>887</v>
       </c>
       <c r="E15" s="16" t="n">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="F15" s="16" t="n">
-        <v>0</v>
+        <v>1367</v>
       </c>
       <c r="G15" s="67" t="n">
-        <v>0</v>
+        <v>-948</v>
       </c>
       <c r="H15" s="67" t="n">
-        <v>0</v>
+        <v>-3330</v>
       </c>
       <c r="I15" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>$300 (A pd) + $180 (L pd) = $480</t>
         </is>
       </c>
     </row>
@@ -6470,27 +6586,31 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C16" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D16" s="16" t="n">
-        <v>0</v>
+        <v>887</v>
       </c>
       <c r="E16" s="16" t="n">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="F16" s="16" t="n">
-        <v>0</v>
+        <v>2087</v>
       </c>
       <c r="G16" s="67" t="n">
-        <v>0</v>
+        <v>-228</v>
       </c>
       <c r="H16" s="67" t="n">
-        <v>0</v>
+        <v>-3558</v>
       </c>
       <c r="I16" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>$200+$200 (A pd) + $300+$500 (L pd) = $1200</t>
         </is>
       </c>
     </row>
@@ -6501,27 +6621,31 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C17" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D17" s="16" t="n">
-        <v>0</v>
+        <v>887</v>
       </c>
       <c r="E17" s="16" t="n">
-        <v>0</v>
+        <v>1550</v>
       </c>
       <c r="F17" s="16" t="n">
-        <v>0</v>
+        <v>2437</v>
       </c>
       <c r="G17" s="67" t="n">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="H17" s="67" t="n">
-        <v>0</v>
+        <v>-3436</v>
       </c>
       <c r="I17" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>A pd $300 9/2 + $500 9/16 + $250 9/29 + L pd $500 9/12 = Total pd $1,550</t>
         </is>
       </c>
     </row>
@@ -6532,27 +6656,31 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D18" s="16" t="n">
-        <v>0</v>
+        <v>887</v>
       </c>
       <c r="E18" s="16" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="F18" s="16" t="n">
-        <v>0</v>
+        <v>1987</v>
       </c>
       <c r="G18" s="67" t="n">
-        <v>0</v>
+        <v>-328</v>
       </c>
       <c r="H18" s="67" t="n">
-        <v>0</v>
+        <v>-3764</v>
       </c>
       <c r="I18" s="19" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>A pd $100 9/30 + $300 10/20 +$300 10/27 = $700 + L pd $400 = $1,100</t>
         </is>
       </c>
     </row>
@@ -6563,27 +6691,31 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D19" s="16" t="n">
-        <v>0</v>
+        <v>1968</v>
       </c>
       <c r="E19" s="16" t="n">
-        <v>0</v>
+        <v>447</v>
       </c>
       <c r="F19" s="16" t="n">
-        <v>0</v>
+        <v>2415</v>
       </c>
       <c r="G19" s="67" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H19" s="67" t="n">
-        <v>0</v>
+        <v>-3664</v>
       </c>
       <c r="I19" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Eff 11/1 (HS: $1968 + T: $347)= $2,315.                       A pd $347 11/4 + $100 11/19 = $447</t>
         </is>
       </c>
     </row>
@@ -6594,27 +6726,31 @@
         </is>
       </c>
       <c r="B20" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="inlineStr"/>
+        <v>2315</v>
+      </c>
+      <c r="C20" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D20" s="16" t="n">
-        <v>0</v>
+        <v>1968</v>
       </c>
       <c r="E20" s="16" t="n">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="F20" s="16" t="n">
-        <v>0</v>
+        <v>2308</v>
       </c>
       <c r="G20" s="67" t="n">
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="H20" s="67" t="n">
-        <v>0</v>
+        <v>-3671</v>
       </c>
       <c r="I20" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>A pd $240 12/1 + $100 12/15 = $340 (2025 Bal due $3,671)</t>
         </is>
       </c>
     </row>
@@ -6802,7 +6938,11 @@
           <t>Property:</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>3908 Irish Setter Dr.</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="6" t="n"/>
       <c r="E4" s="6" t="n"/>
@@ -6812,7 +6952,11 @@
         </is>
       </c>
       <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="inlineStr"/>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Gabrielle Owens</t>
+        </is>
+      </c>
       <c r="I4" s="5" t="n"/>
     </row>
     <row r="5" ht="19" customHeight="1">
@@ -6920,17 +7064,21 @@
         </is>
       </c>
       <c r="B9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C9" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D9" s="16" t="n">
-        <v>0</v>
+        <v>2142</v>
       </c>
       <c r="E9" s="16" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G9" s="67" t="n">
         <v>0</v>
@@ -6938,11 +7086,7 @@
       <c r="H9" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I9" s="18" t="inlineStr"/>
     </row>
     <row r="10" ht="22" customHeight="1">
       <c r="A10" s="13" t="inlineStr">
@@ -6951,17 +7095,21 @@
         </is>
       </c>
       <c r="B10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C10" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D10" s="16" t="n">
-        <v>0</v>
+        <v>2142</v>
       </c>
       <c r="E10" s="16" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G10" s="67" t="n">
         <v>0</v>
@@ -6969,11 +7117,7 @@
       <c r="H10" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I10" s="18" t="inlineStr"/>
     </row>
     <row r="11" ht="22" customHeight="1">
       <c r="A11" s="13" t="inlineStr">
@@ -6982,17 +7126,21 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D11" s="16" t="n">
-        <v>0</v>
+        <v>2142</v>
       </c>
       <c r="E11" s="16" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G11" s="67" t="n">
         <v>0</v>
@@ -7000,11 +7148,7 @@
       <c r="H11" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I11" s="18" t="inlineStr"/>
     </row>
     <row r="12" ht="22" customHeight="1">
       <c r="A12" s="13" t="inlineStr">
@@ -7013,17 +7157,21 @@
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D12" s="16" t="n">
-        <v>0</v>
+        <v>2142</v>
       </c>
       <c r="E12" s="16" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G12" s="67" t="n">
         <v>0</v>
@@ -7031,11 +7179,7 @@
       <c r="H12" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I12" s="18" t="inlineStr"/>
     </row>
     <row r="13" ht="22" customHeight="1">
       <c r="A13" s="13" t="inlineStr">
@@ -7044,17 +7188,21 @@
         </is>
       </c>
       <c r="B13" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C13" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D13" s="16" t="n">
-        <v>0</v>
+        <v>2142</v>
       </c>
       <c r="E13" s="16" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="F13" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G13" s="67" t="n">
         <v>0</v>
@@ -7062,11 +7210,7 @@
       <c r="H13" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I13" s="18" t="inlineStr"/>
     </row>
     <row r="14" ht="22" customHeight="1">
       <c r="A14" s="13" t="inlineStr">
@@ -7075,17 +7219,21 @@
         </is>
       </c>
       <c r="B14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C14" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D14" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="E14" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G14" s="67" t="n">
         <v>0</v>
@@ -7095,7 +7243,7 @@
       </c>
       <c r="I14" s="18" t="inlineStr">
         <is>
-          <t>Missing data</t>
+          <t>Eff 6/1 FWHS: $2485</t>
         </is>
       </c>
     </row>
@@ -7106,17 +7254,21 @@
         </is>
       </c>
       <c r="B15" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C15" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D15" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="E15" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F15" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G15" s="67" t="n">
         <v>0</v>
@@ -7124,11 +7276,7 @@
       <c r="H15" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I15" s="18" t="inlineStr"/>
     </row>
     <row r="16" ht="22" customHeight="1">
       <c r="A16" s="13" t="inlineStr">
@@ -7137,17 +7285,21 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C16" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D16" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="E16" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F16" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G16" s="67" t="n">
         <v>0</v>
@@ -7155,11 +7307,7 @@
       <c r="H16" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I16" s="18" t="inlineStr"/>
     </row>
     <row r="17" ht="22" customHeight="1">
       <c r="A17" s="13" t="inlineStr">
@@ -7168,17 +7316,21 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C17" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D17" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="E17" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G17" s="67" t="n">
         <v>0</v>
@@ -7186,11 +7338,7 @@
       <c r="H17" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I17" s="18" t="inlineStr"/>
     </row>
     <row r="18" ht="22" customHeight="1">
       <c r="A18" s="13" t="inlineStr">
@@ -7199,17 +7347,21 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D18" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="E18" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G18" s="67" t="n">
         <v>0</v>
@@ -7217,11 +7369,7 @@
       <c r="H18" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I18" s="19" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I18" s="19" t="inlineStr"/>
     </row>
     <row r="19" ht="22" customHeight="1">
       <c r="A19" s="13" t="inlineStr">
@@ -7230,17 +7378,21 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D19" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="E19" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G19" s="67" t="n">
         <v>0</v>
@@ -7248,11 +7400,7 @@
       <c r="H19" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I19" s="18" t="inlineStr"/>
     </row>
     <row r="20" ht="22" customHeight="1">
       <c r="A20" s="13" t="inlineStr">
@@ -7261,17 +7409,21 @@
         </is>
       </c>
       <c r="B20" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="inlineStr"/>
+        <v>2485</v>
+      </c>
+      <c r="C20" s="15" t="inlineStr">
+        <is>
+          <t>Fort Worth</t>
+        </is>
+      </c>
       <c r="D20" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="E20" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="16" t="n">
-        <v>0</v>
+        <v>2485</v>
       </c>
       <c r="G20" s="67" t="n">
         <v>0</v>
@@ -7279,11 +7431,7 @@
       <c r="H20" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I20" s="18" t="inlineStr"/>
     </row>
     <row r="21" ht="22" customHeight="1" thickBot="1">
       <c r="A21" s="20" t="inlineStr">
@@ -7595,17 +7743,21 @@
         </is>
       </c>
       <c r="B9" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="inlineStr"/>
+        <v>2350</v>
+      </c>
+      <c r="C9" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D9" s="16" t="n">
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="E9" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F9" s="16" t="n">
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="G9" s="67" t="n">
         <v>0</v>
@@ -7613,11 +7765,7 @@
       <c r="H9" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I9" s="18" t="inlineStr"/>
     </row>
     <row r="10" ht="22" customHeight="1">
       <c r="A10" s="13" t="inlineStr">
@@ -7626,17 +7774,21 @@
         </is>
       </c>
       <c r="B10" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="inlineStr"/>
+        <v>2350</v>
+      </c>
+      <c r="C10" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D10" s="16" t="n">
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="E10" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="16" t="n">
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="G10" s="67" t="n">
         <v>0</v>
@@ -7644,11 +7796,7 @@
       <c r="H10" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I10" s="18" t="inlineStr"/>
     </row>
     <row r="11" ht="22" customHeight="1">
       <c r="A11" s="13" t="inlineStr">
@@ -7657,17 +7805,21 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="inlineStr"/>
+        <v>2350</v>
+      </c>
+      <c r="C11" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D11" s="16" t="n">
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="E11" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="16" t="n">
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="G11" s="67" t="n">
         <v>0</v>
@@ -7675,11 +7827,7 @@
       <c r="H11" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I11" s="18" t="inlineStr"/>
     </row>
     <row r="12" ht="22" customHeight="1">
       <c r="A12" s="13" t="inlineStr">
@@ -7688,17 +7836,21 @@
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="inlineStr"/>
+        <v>2350</v>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>Tarrant County</t>
+        </is>
+      </c>
       <c r="D12" s="16" t="n">
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="E12" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="16" t="n">
-        <v>0</v>
+        <v>2350</v>
       </c>
       <c r="G12" s="67" t="n">
         <v>0</v>
@@ -7706,11 +7858,7 @@
       <c r="H12" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="18" t="inlineStr">
-        <is>
-          <t>Missing data</t>
-        </is>
-      </c>
+      <c r="I12" s="18" t="inlineStr"/>
     </row>
     <row r="13" ht="22" customHeight="1">
       <c r="A13" s="13" t="inlineStr">

</xml_diff>